<commit_message>
[AM] Work on Country Code Adjustments for Dynamic Dataset
</commit_message>
<xml_diff>
--- a/pyeconlab/trade/dataset/NBERFeenstraWTF/meta/xlsx/exporter-eiso3n_intertemporal_countrycode_adjustments.xlsx
+++ b/pyeconlab/trade/dataset/NBERFeenstraWTF/meta/xlsx/exporter-eiso3n_intertemporal_countrycode_adjustments.xlsx
@@ -1086,10 +1086,10 @@
   <dimension ref="A1:AW49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3270" ySplit="555" topLeftCell="AG22" activePane="bottomRight"/>
+      <pane xSplit="3270" ySplit="555" topLeftCell="AR1" activePane="bottomRight"/>
       <selection pane="topRight" activeCell="AU1" sqref="AU1:AU1048576"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AT54" sqref="AT54"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="AT6" sqref="AT6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>